<commit_message>
implement parsing for multiple data types
</commit_message>
<xml_diff>
--- a/spec/fixtures/test_spreadsheet.xlsx
+++ b/spec/fixtures/test_spreadsheet.xlsx
@@ -113,11 +113,12 @@
     <numFmt numFmtId="166" formatCode="[$USD]0.00"/>
     <numFmt numFmtId="167" formatCode="[$€-2]0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -137,12 +138,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -199,19 +194,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,7 +225,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D5"/>
@@ -328,13 +323,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -375,12 +370,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="21.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>123456</v>
+        <v>123.456</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>39507</v>
@@ -423,7 +418,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>